<commit_message>
User Agent added to header
</commit_message>
<xml_diff>
--- a/TeamTime.xlsx
+++ b/TeamTime.xlsx
@@ -95,7 +95,7 @@
     <t>53.741</t>
   </si>
   <si>
-    <t>47.174</t>
+    <t>47.018</t>
   </si>
   <si>
     <t>01:00.825</t>
@@ -107,7 +107,7 @@
     <t>01:03.745</t>
   </si>
   <si>
-    <t>01:11.487</t>
+    <t>01:04.030</t>
   </si>
   <si>
     <t>01:09.678</t>
@@ -293,7 +293,7 @@
     <t>01:11.026</t>
   </si>
   <si>
-    <t>26.365</t>
+    <t>26.291</t>
   </si>
   <si>
     <t>29.504</t>
@@ -332,10 +332,10 @@
     <t>54.688</t>
   </si>
   <si>
-    <t>47.508</t>
-  </si>
-  <si>
-    <t>01:02.041</t>
+    <t>47.321</t>
+  </si>
+  <si>
+    <t>01:01.548</t>
   </si>
   <si>
     <t>57.978</t>
@@ -380,10 +380,10 @@
     <t>Domi_TM time</t>
   </si>
   <si>
-    <t>35.116</t>
-  </si>
-  <si>
-    <t>26.008</t>
+    <t>35.115</t>
+  </si>
+  <si>
+    <t>25.943</t>
   </si>
   <si>
     <t>29.296</t>
@@ -443,7 +443,7 @@
     <t>35.384</t>
   </si>
   <si>
-    <t>26.515</t>
+    <t>26.355</t>
   </si>
   <si>
     <t>29.688</t>
@@ -518,7 +518,7 @@
     <t>31.165</t>
   </si>
   <si>
-    <t>39.456</t>
+    <t>39.383</t>
   </si>
   <si>
     <t>31.664</t>
@@ -671,7 +671,7 @@
     <t>01:10.836</t>
   </si>
   <si>
-    <t>01:18.821</t>
+    <t>01:11.988</t>
   </si>
   <si>
     <t>01:18.185</t>
@@ -1095,37 +1095,37 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2">
-        <v>1276</v>
+        <v>1281</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
       </c>
       <c r="F2">
-        <v>3027</v>
+        <v>3037</v>
       </c>
       <c r="G2" t="s">
         <v>52</v>
       </c>
       <c r="H2">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="I2" t="s">
         <v>72</v>
       </c>
       <c r="J2">
-        <v>3027</v>
+        <v>3037</v>
       </c>
       <c r="K2" t="s">
         <v>52</v>
       </c>
       <c r="L2">
-        <v>953</v>
+        <v>957</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1139,31 +1139,31 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>1340</v>
+        <v>1346</v>
       </c>
       <c r="E3" t="s">
         <v>33</v>
       </c>
       <c r="F3">
-        <v>5781</v>
+        <v>5792</v>
       </c>
       <c r="G3" t="s">
         <v>53</v>
       </c>
       <c r="H3">
-        <v>1255</v>
+        <v>1261</v>
       </c>
       <c r="I3" t="s">
         <v>73</v>
       </c>
       <c r="J3">
-        <v>2695</v>
+        <v>2080</v>
       </c>
       <c r="K3" t="s">
         <v>92</v>
       </c>
       <c r="L3">
-        <v>920</v>
+        <v>924</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1171,37 +1171,37 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>1385</v>
+        <v>1390</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4">
-        <v>2103</v>
+        <v>2110</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4">
-        <v>5476</v>
+        <v>5488</v>
       </c>
       <c r="G4" t="s">
         <v>54</v>
       </c>
       <c r="H4">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="I4" t="s">
         <v>74</v>
       </c>
       <c r="J4">
-        <v>1491</v>
+        <v>1496</v>
       </c>
       <c r="K4" t="s">
         <v>93</v>
       </c>
       <c r="L4">
-        <v>1173</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1209,37 +1209,37 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2195</v>
+        <v>2198</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5">
-        <v>4770</v>
+        <v>4783</v>
       </c>
       <c r="E5" t="s">
         <v>35</v>
       </c>
       <c r="F5">
-        <v>4472</v>
+        <v>4485</v>
       </c>
       <c r="G5" t="s">
         <v>55</v>
       </c>
       <c r="H5">
-        <v>1499</v>
+        <v>1504</v>
       </c>
       <c r="I5" t="s">
         <v>75</v>
       </c>
       <c r="J5">
-        <v>1426</v>
+        <v>1431</v>
       </c>
       <c r="K5" t="s">
         <v>94</v>
       </c>
       <c r="L5">
-        <v>1706</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1247,37 +1247,37 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6">
-        <v>2430</v>
+        <v>2438</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
       </c>
       <c r="F6">
-        <v>5177</v>
+        <v>5191</v>
       </c>
       <c r="G6" t="s">
         <v>56</v>
       </c>
       <c r="H6">
-        <v>744</v>
+        <v>749</v>
       </c>
       <c r="I6" t="s">
         <v>76</v>
       </c>
       <c r="J6">
-        <v>2541</v>
+        <v>2550</v>
       </c>
       <c r="K6" t="s">
         <v>95</v>
       </c>
       <c r="L6">
-        <v>1181</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1285,37 +1285,37 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7">
-        <v>2336</v>
+        <v>2345</v>
       </c>
       <c r="E7" t="s">
         <v>37</v>
       </c>
       <c r="F7">
-        <v>3860</v>
+        <v>3866</v>
       </c>
       <c r="G7" t="s">
         <v>57</v>
       </c>
       <c r="H7">
-        <v>2190</v>
+        <v>2200</v>
       </c>
       <c r="I7" t="s">
         <v>77</v>
       </c>
       <c r="J7">
-        <v>1416</v>
+        <v>1421</v>
       </c>
       <c r="K7" t="s">
         <v>96</v>
       </c>
       <c r="L7">
-        <v>1422</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1323,7 +1323,7 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -1335,25 +1335,25 @@
         <v>38</v>
       </c>
       <c r="F8">
-        <v>3818</v>
+        <v>3830</v>
       </c>
       <c r="G8" t="s">
         <v>58</v>
       </c>
       <c r="H8">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="I8" t="s">
         <v>78</v>
       </c>
       <c r="J8">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="K8" t="s">
         <v>97</v>
       </c>
       <c r="L8">
-        <v>1321</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1367,7 +1367,7 @@
         <v>19</v>
       </c>
       <c r="D9">
-        <v>2477</v>
+        <v>2485</v>
       </c>
       <c r="E9" t="s">
         <v>39</v>
@@ -1379,19 +1379,19 @@
         <v>59</v>
       </c>
       <c r="H9">
-        <v>1476</v>
+        <v>1481</v>
       </c>
       <c r="I9" t="s">
         <v>79</v>
       </c>
       <c r="J9">
-        <v>1908</v>
+        <v>1916</v>
       </c>
       <c r="K9" t="s">
         <v>98</v>
       </c>
       <c r="L9">
-        <v>1193</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1399,37 +1399,37 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="D10">
-        <v>1595</v>
+        <v>1599</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
       </c>
       <c r="F10">
-        <v>5846</v>
+        <v>5854</v>
       </c>
       <c r="G10" t="s">
         <v>60</v>
       </c>
       <c r="H10">
-        <v>1086</v>
+        <v>1091</v>
       </c>
       <c r="I10" t="s">
         <v>80</v>
       </c>
       <c r="J10">
-        <v>1136</v>
+        <v>1140</v>
       </c>
       <c r="K10" t="s">
         <v>99</v>
       </c>
       <c r="L10">
-        <v>809</v>
+        <v>813</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1437,37 +1437,37 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11">
-        <v>2467</v>
+        <v>2476</v>
       </c>
       <c r="E11" t="s">
         <v>41</v>
       </c>
       <c r="F11">
-        <v>5798</v>
+        <v>5813</v>
       </c>
       <c r="G11" t="s">
         <v>61</v>
       </c>
       <c r="H11">
-        <v>1983</v>
+        <v>1994</v>
       </c>
       <c r="I11" t="s">
         <v>81</v>
       </c>
       <c r="J11">
-        <v>1177</v>
+        <v>1181</v>
       </c>
       <c r="K11" t="s">
         <v>100</v>
       </c>
       <c r="L11">
-        <v>1104</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1481,7 +1481,7 @@
         <v>22</v>
       </c>
       <c r="D12">
-        <v>1731</v>
+        <v>1736</v>
       </c>
       <c r="E12" t="s">
         <v>42</v>
@@ -1493,19 +1493,19 @@
         <v>62</v>
       </c>
       <c r="H12">
-        <v>1373</v>
+        <v>1376</v>
       </c>
       <c r="I12" t="s">
         <v>82</v>
       </c>
       <c r="J12">
-        <v>1441</v>
+        <v>1444</v>
       </c>
       <c r="K12" t="s">
         <v>101</v>
       </c>
       <c r="L12">
-        <v>983</v>
+        <v>985</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1513,13 +1513,13 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13">
-        <v>2637</v>
+        <v>2648</v>
       </c>
       <c r="E13" t="s">
         <v>43</v>
@@ -1531,19 +1531,19 @@
         <v>63</v>
       </c>
       <c r="H13">
-        <v>1744</v>
+        <v>1748</v>
       </c>
       <c r="I13" t="s">
         <v>83</v>
       </c>
       <c r="J13">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="K13" t="s">
         <v>102</v>
       </c>
       <c r="L13">
-        <v>1000</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1551,37 +1551,37 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14">
-        <v>1383</v>
+        <v>1386</v>
       </c>
       <c r="E14" t="s">
         <v>44</v>
       </c>
       <c r="F14">
-        <v>8310</v>
+        <v>8327</v>
       </c>
       <c r="G14" t="s">
         <v>64</v>
       </c>
       <c r="H14">
-        <v>1455</v>
+        <v>1458</v>
       </c>
       <c r="I14" t="s">
         <v>84</v>
       </c>
       <c r="J14">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="K14" t="s">
         <v>103</v>
       </c>
       <c r="L14">
-        <v>872</v>
+        <v>874</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1589,37 +1589,37 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
       <c r="D15">
-        <v>1496</v>
+        <v>1503</v>
       </c>
       <c r="E15" t="s">
         <v>45</v>
       </c>
       <c r="F15">
-        <v>2109</v>
+        <v>2118</v>
       </c>
       <c r="G15" t="s">
         <v>65</v>
       </c>
       <c r="H15">
-        <v>1927</v>
+        <v>1934</v>
       </c>
       <c r="I15" t="s">
         <v>85</v>
       </c>
       <c r="J15">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="K15" t="s">
         <v>104</v>
       </c>
       <c r="L15">
-        <v>841</v>
+        <v>845</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1627,37 +1627,37 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>1494</v>
+        <v>953</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
       </c>
       <c r="D16">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="E16" t="s">
         <v>46</v>
       </c>
       <c r="F16">
-        <v>1390</v>
+        <v>1393</v>
       </c>
       <c r="G16" t="s">
         <v>66</v>
       </c>
       <c r="H16">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="I16" t="s">
         <v>86</v>
       </c>
       <c r="J16">
-        <v>3482</v>
+        <v>2150</v>
       </c>
       <c r="K16" t="s">
         <v>105</v>
       </c>
       <c r="L16">
-        <v>1052</v>
+        <v>909</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1665,37 +1665,37 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
       </c>
       <c r="D17">
-        <v>6599</v>
+        <v>6611</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
       </c>
       <c r="F17">
-        <v>8622</v>
+        <v>8638</v>
       </c>
       <c r="G17" t="s">
         <v>67</v>
       </c>
       <c r="H17">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="I17" t="s">
         <v>87</v>
       </c>
       <c r="J17">
-        <v>2483</v>
+        <v>1349</v>
       </c>
       <c r="K17" t="s">
         <v>106</v>
       </c>
       <c r="L17">
-        <v>1269</v>
+        <v>892</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1703,37 +1703,37 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
       </c>
       <c r="D18">
-        <v>7407</v>
+        <v>7418</v>
       </c>
       <c r="E18" t="s">
         <v>48</v>
       </c>
       <c r="F18">
-        <v>3145</v>
+        <v>3157</v>
       </c>
       <c r="G18" t="s">
         <v>68</v>
       </c>
       <c r="H18">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="I18" t="s">
         <v>88</v>
       </c>
       <c r="J18">
-        <v>1756</v>
+        <v>1760</v>
       </c>
       <c r="K18" t="s">
         <v>107</v>
       </c>
       <c r="L18">
-        <v>1066</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1741,37 +1741,37 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
       </c>
       <c r="D19">
-        <v>2588</v>
+        <v>2599</v>
       </c>
       <c r="E19" t="s">
         <v>49</v>
       </c>
       <c r="F19">
-        <v>6024</v>
+        <v>6036</v>
       </c>
       <c r="G19" t="s">
         <v>69</v>
       </c>
       <c r="H19">
-        <v>3048</v>
+        <v>3059</v>
       </c>
       <c r="I19" t="s">
         <v>89</v>
       </c>
       <c r="J19">
-        <v>1186</v>
+        <v>1190</v>
       </c>
       <c r="K19" t="s">
         <v>108</v>
       </c>
       <c r="L19">
-        <v>1333</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1779,37 +1779,37 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>19999</v>
+        <v>317</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
       </c>
       <c r="D20">
-        <v>1753</v>
+        <v>1758</v>
       </c>
       <c r="E20" t="s">
         <v>50</v>
       </c>
       <c r="F20">
-        <v>4993</v>
+        <v>5014</v>
       </c>
       <c r="G20" t="s">
         <v>70</v>
       </c>
       <c r="H20">
-        <v>1077</v>
+        <v>1081</v>
       </c>
       <c r="I20" t="s">
         <v>90</v>
       </c>
       <c r="J20">
-        <v>960</v>
+        <v>965</v>
       </c>
       <c r="K20" t="s">
         <v>109</v>
       </c>
       <c r="L20">
-        <v>1263</v>
+        <v>787</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1823,19 +1823,19 @@
         <v>31</v>
       </c>
       <c r="D21">
-        <v>3296</v>
+        <v>3304</v>
       </c>
       <c r="E21" t="s">
         <v>51</v>
       </c>
       <c r="F21">
-        <v>2934</v>
+        <v>2941</v>
       </c>
       <c r="G21" t="s">
         <v>71</v>
       </c>
       <c r="H21">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="I21" t="s">
         <v>91</v>
@@ -1847,7 +1847,7 @@
         <v>110</v>
       </c>
       <c r="L21">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -1920,37 +1920,37 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1258</v>
+        <v>1239</v>
       </c>
       <c r="C2" t="s">
         <v>121</v>
       </c>
       <c r="D2">
-        <v>5015</v>
+        <v>5032</v>
       </c>
       <c r="E2" t="s">
         <v>141</v>
       </c>
       <c r="F2">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G2" t="s">
         <v>161</v>
       </c>
       <c r="H2">
-        <v>2624</v>
+        <v>2634</v>
       </c>
       <c r="I2" t="s">
         <v>180</v>
       </c>
       <c r="J2">
-        <v>5191</v>
+        <v>5209</v>
       </c>
       <c r="K2" t="s">
         <v>200</v>
       </c>
       <c r="L2">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1958,25 +1958,25 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>707</v>
+        <v>526</v>
       </c>
       <c r="C3" t="s">
         <v>122</v>
       </c>
       <c r="D3">
-        <v>4845</v>
+        <v>2621</v>
       </c>
       <c r="E3" t="s">
         <v>142</v>
       </c>
       <c r="F3">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c r="G3" t="s">
         <v>162</v>
       </c>
       <c r="H3">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="I3" t="s">
         <v>181</v>
@@ -1988,7 +1988,7 @@
         <v>201</v>
       </c>
       <c r="L3">
-        <v>694</v>
+        <v>635</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1996,13 +1996,13 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>778</v>
+        <v>782</v>
       </c>
       <c r="C4" t="s">
         <v>123</v>
       </c>
       <c r="D4">
-        <v>2658</v>
+        <v>2664</v>
       </c>
       <c r="E4" t="s">
         <v>143</v>
@@ -2014,19 +2014,19 @@
         <v>163</v>
       </c>
       <c r="H4">
-        <v>1548</v>
+        <v>1555</v>
       </c>
       <c r="I4" t="s">
         <v>182</v>
       </c>
       <c r="J4">
-        <v>1735</v>
+        <v>1743</v>
       </c>
       <c r="K4" t="s">
         <v>202</v>
       </c>
       <c r="L4">
-        <v>820</v>
+        <v>823</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2034,25 +2034,25 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
       </c>
       <c r="D5">
-        <v>3273</v>
+        <v>3280</v>
       </c>
       <c r="E5" t="s">
         <v>144</v>
       </c>
       <c r="F5">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G5" t="s">
         <v>164</v>
       </c>
       <c r="H5">
-        <v>8372</v>
+        <v>8394</v>
       </c>
       <c r="I5" t="s">
         <v>183</v>
@@ -2064,7 +2064,7 @@
         <v>203</v>
       </c>
       <c r="L5">
-        <v>1250</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2072,25 +2072,25 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>1916</v>
+        <v>1926</v>
       </c>
       <c r="C6" t="s">
         <v>125</v>
       </c>
       <c r="D6">
-        <v>1981</v>
+        <v>1991</v>
       </c>
       <c r="E6" t="s">
         <v>145</v>
       </c>
       <c r="F6">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G6" t="s">
         <v>165</v>
       </c>
       <c r="H6">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I6" t="s">
         <v>184</v>
@@ -2102,7 +2102,7 @@
         <v>204</v>
       </c>
       <c r="L6">
-        <v>851</v>
+        <v>855</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2110,25 +2110,25 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>2721</v>
+        <v>2730</v>
       </c>
       <c r="C7" t="s">
         <v>126</v>
       </c>
       <c r="D7">
-        <v>2663</v>
+        <v>2673</v>
       </c>
       <c r="E7" t="s">
         <v>146</v>
       </c>
       <c r="F7">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="G7" t="s">
         <v>166</v>
       </c>
       <c r="H7">
-        <v>1454</v>
+        <v>1459</v>
       </c>
       <c r="I7" t="s">
         <v>185</v>
@@ -2140,7 +2140,7 @@
         <v>205</v>
       </c>
       <c r="L7">
-        <v>1675</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2154,31 +2154,31 @@
         <v>127</v>
       </c>
       <c r="D8">
-        <v>2840</v>
+        <v>2846</v>
       </c>
       <c r="E8" t="s">
         <v>147</v>
       </c>
       <c r="F8">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G8" t="s">
         <v>167</v>
       </c>
       <c r="H8">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I8" t="s">
         <v>186</v>
       </c>
       <c r="J8">
-        <v>4621</v>
+        <v>4632</v>
       </c>
       <c r="K8" t="s">
         <v>206</v>
       </c>
       <c r="L8">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2186,37 +2186,37 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>1602</v>
+        <v>1607</v>
       </c>
       <c r="C9" t="s">
         <v>128</v>
       </c>
       <c r="D9">
-        <v>1927</v>
+        <v>1935</v>
       </c>
       <c r="E9" t="s">
         <v>148</v>
       </c>
       <c r="F9">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="G9" t="s">
         <v>168</v>
       </c>
       <c r="H9">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="I9" t="s">
         <v>187</v>
       </c>
       <c r="J9">
-        <v>2961</v>
+        <v>2965</v>
       </c>
       <c r="K9" t="s">
         <v>207</v>
       </c>
       <c r="L9">
-        <v>903</v>
+        <v>905</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2224,37 +2224,37 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>3191</v>
+        <v>3196</v>
       </c>
       <c r="C10" t="s">
         <v>129</v>
       </c>
       <c r="D10">
-        <v>2620</v>
+        <v>2626</v>
       </c>
       <c r="E10" t="s">
         <v>149</v>
       </c>
       <c r="F10">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="G10" t="s">
         <v>169</v>
       </c>
       <c r="H10">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="I10" t="s">
         <v>188</v>
       </c>
       <c r="J10">
-        <v>2808</v>
+        <v>2814</v>
       </c>
       <c r="K10" t="s">
         <v>208</v>
       </c>
       <c r="L10">
-        <v>1349</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2262,37 +2262,37 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>3977</v>
+        <v>3984</v>
       </c>
       <c r="C11" t="s">
         <v>130</v>
       </c>
       <c r="D11">
-        <v>4114</v>
+        <v>4123</v>
       </c>
       <c r="E11" t="s">
         <v>150</v>
       </c>
       <c r="F11">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="G11" t="s">
         <v>170</v>
       </c>
       <c r="H11">
-        <v>1160</v>
+        <v>1164</v>
       </c>
       <c r="I11" t="s">
         <v>189</v>
       </c>
       <c r="J11">
-        <v>6037</v>
+        <v>6053</v>
       </c>
       <c r="K11" t="s">
         <v>209</v>
       </c>
       <c r="L11">
-        <v>1930</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2300,13 +2300,13 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>3407</v>
+        <v>3415</v>
       </c>
       <c r="C12" t="s">
         <v>131</v>
       </c>
       <c r="D12">
-        <v>1679</v>
+        <v>1684</v>
       </c>
       <c r="E12" t="s">
         <v>151</v>
@@ -2318,19 +2318,19 @@
         <v>171</v>
       </c>
       <c r="H12">
-        <v>1728</v>
+        <v>1733</v>
       </c>
       <c r="I12" t="s">
         <v>190</v>
       </c>
       <c r="J12">
-        <v>7648</v>
+        <v>7663</v>
       </c>
       <c r="K12" t="s">
         <v>210</v>
       </c>
       <c r="L12">
-        <v>1179</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2338,19 +2338,19 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>2715</v>
+        <v>2726</v>
       </c>
       <c r="C13" t="s">
         <v>132</v>
       </c>
       <c r="D13">
-        <v>1285</v>
+        <v>1289</v>
       </c>
       <c r="E13" t="s">
         <v>152</v>
       </c>
       <c r="F13">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="G13" t="s">
         <v>172</v>
@@ -2362,13 +2362,13 @@
         <v>191</v>
       </c>
       <c r="J13">
-        <v>4076</v>
+        <v>4084</v>
       </c>
       <c r="K13" t="s">
         <v>211</v>
       </c>
       <c r="L13">
-        <v>774</v>
+        <v>776</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2382,19 +2382,19 @@
         <v>133</v>
       </c>
       <c r="D14">
-        <v>1796</v>
+        <v>1800</v>
       </c>
       <c r="E14" t="s">
         <v>153</v>
       </c>
       <c r="F14">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="G14" t="s">
         <v>173</v>
       </c>
       <c r="H14">
-        <v>1887</v>
+        <v>1891</v>
       </c>
       <c r="I14" t="s">
         <v>192</v>
@@ -2406,7 +2406,7 @@
         <v>212</v>
       </c>
       <c r="L14">
-        <v>1450</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2414,25 +2414,25 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>2338</v>
+        <v>2347</v>
       </c>
       <c r="C15" t="s">
         <v>134</v>
       </c>
       <c r="D15">
-        <v>2274</v>
+        <v>2283</v>
       </c>
       <c r="E15" t="s">
         <v>154</v>
       </c>
       <c r="F15">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="G15" t="s">
         <v>174</v>
       </c>
       <c r="H15">
-        <v>6506</v>
+        <v>6525</v>
       </c>
       <c r="I15" t="s">
         <v>193</v>
@@ -2444,7 +2444,7 @@
         <v>213</v>
       </c>
       <c r="L15">
-        <v>1691</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2452,25 +2452,25 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>9815</v>
+        <v>9832</v>
       </c>
       <c r="C16" t="s">
         <v>135</v>
       </c>
       <c r="D16">
-        <v>2471</v>
+        <v>2478</v>
       </c>
       <c r="E16" t="s">
         <v>155</v>
       </c>
       <c r="F16">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="G16" t="s">
         <v>86</v>
       </c>
       <c r="H16">
-        <v>2740</v>
+        <v>2750</v>
       </c>
       <c r="I16" t="s">
         <v>194</v>
@@ -2482,7 +2482,7 @@
         <v>214</v>
       </c>
       <c r="L16">
-        <v>2019</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2490,25 +2490,25 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>9143</v>
+        <v>9159</v>
       </c>
       <c r="C17" t="s">
         <v>136</v>
       </c>
       <c r="D17">
-        <v>2669</v>
+        <v>2671</v>
       </c>
       <c r="E17" t="s">
         <v>156</v>
       </c>
       <c r="F17">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="G17" t="s">
         <v>175</v>
       </c>
       <c r="H17">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="I17" t="s">
         <v>195</v>
@@ -2520,7 +2520,7 @@
         <v>215</v>
       </c>
       <c r="L17">
-        <v>1292</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -2528,13 +2528,13 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>5673</v>
+        <v>5683</v>
       </c>
       <c r="C18" t="s">
         <v>137</v>
       </c>
       <c r="D18">
-        <v>3130</v>
+        <v>3142</v>
       </c>
       <c r="E18" t="s">
         <v>157</v>
@@ -2546,7 +2546,7 @@
         <v>176</v>
       </c>
       <c r="H18">
-        <v>2552</v>
+        <v>2559</v>
       </c>
       <c r="I18" t="s">
         <v>196</v>
@@ -2558,7 +2558,7 @@
         <v>216</v>
       </c>
       <c r="L18">
-        <v>1916</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2566,25 +2566,25 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>7839</v>
+        <v>7857</v>
       </c>
       <c r="C19" t="s">
         <v>138</v>
       </c>
       <c r="D19">
-        <v>2435</v>
+        <v>2444</v>
       </c>
       <c r="E19" t="s">
         <v>158</v>
       </c>
       <c r="F19">
-        <v>916</v>
+        <v>920</v>
       </c>
       <c r="G19" t="s">
         <v>177</v>
       </c>
       <c r="H19">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="I19" t="s">
         <v>197</v>
@@ -2596,7 +2596,7 @@
         <v>217</v>
       </c>
       <c r="L19">
-        <v>1333</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -2604,37 +2604,37 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>7097</v>
+        <v>7119</v>
       </c>
       <c r="C20" t="s">
         <v>139</v>
       </c>
       <c r="D20">
-        <v>1446</v>
+        <v>1451</v>
       </c>
       <c r="E20" t="s">
         <v>159</v>
       </c>
       <c r="F20">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="G20" t="s">
         <v>178</v>
       </c>
       <c r="H20">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I20" t="s">
         <v>198</v>
       </c>
       <c r="J20">
-        <v>29999</v>
+        <v>19999</v>
       </c>
       <c r="K20" t="s">
         <v>218</v>
       </c>
       <c r="L20">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2642,25 +2642,25 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>1940</v>
+        <v>1948</v>
       </c>
       <c r="C21" t="s">
         <v>140</v>
       </c>
       <c r="D21">
-        <v>2240</v>
+        <v>2245</v>
       </c>
       <c r="E21" t="s">
         <v>160</v>
       </c>
       <c r="F21">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="G21" t="s">
         <v>179</v>
       </c>
       <c r="H21">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="I21" t="s">
         <v>199</v>
@@ -2672,7 +2672,7 @@
         <v>219</v>
       </c>
       <c r="L21">
-        <v>1194</v>
+        <v>1198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>